<commit_message>
Update Klasifikasi Tingkat Kemiskinan di Indonesia.xlsx
ok
</commit_message>
<xml_diff>
--- a/Klasifikasi Tingkat Kemiskinan di Indonesia.xlsx
+++ b/Klasifikasi Tingkat Kemiskinan di Indonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANNA\BANK SOAL UJIAN\AI\2024-20205\kemiskinan\dataset-kemiskinan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{222051DE-DDFA-4A25-BC9C-39113547084B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799E405C-314F-45C9-8F9F-D1FC3209B39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7ED517F8-17D7-409C-B471-B81B42501263}"/>
   </bookViews>
@@ -2775,7 +2775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4BE5DA-E2FF-48A2-BA4A-5FC289FDC028}">
   <dimension ref="A1:M515"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>